<commit_message>
update code and data
</commit_message>
<xml_diff>
--- a/party_support.xlsx
+++ b/party_support.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\My projects\scratchpad\party_support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C9C759-6B0F-4D9F-9B77-14A94008462C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3334FF8C-FB17-4FA4-AD19-1F331BA6AEAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4B62CDA0-0208-4958-8E45-C4D2A9261E0D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4B62CDA0-0208-4958-8E45-C4D2A9261E0D}"/>
   </bookViews>
   <sheets>
     <sheet name="ndi_crrc" sheetId="1" r:id="rId1"/>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4E3216-E01E-4ACB-A1A2-82C046BF6034}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F197" sqref="A197:XFD201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4102,7 +4102,7 @@
         <v>14</v>
       </c>
       <c r="F181" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
@@ -4202,7 +4202,7 @@
         <v>14</v>
       </c>
       <c r="F186" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -4520,7 +4520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A06D1A-EF84-4B6E-91B4-460275DCC550}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>